<commit_message>
Import de proprietaires opérationnel
</commit_message>
<xml_diff>
--- a/admin_interface/initData/users.xlsx
+++ b/admin_interface/initData/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perre\eclipse-workspace\Django\les_grandes_oreilles\admin_interface\initData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CE265B-A445-426B-9F92-F4FFB910A1E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152AD4D5-659B-49CB-93EA-0D7F6B4C5728}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDBA8DEB-44BB-44BA-ABA8-A3259AD206CD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -116,28 +116,28 @@
     <t>PerreautBis</t>
   </si>
   <si>
-    <t>clementine.perreautbis</t>
-  </si>
-  <si>
-    <t>laurie.callo</t>
-  </si>
-  <si>
-    <t>charles.chaplin</t>
-  </si>
-  <si>
-    <t>sabine.gauger</t>
-  </si>
-  <si>
-    <t>dexter.serie</t>
-  </si>
-  <si>
-    <t>chloe.machado</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>perreautbis.clementine</t>
+  </si>
+  <si>
+    <t>callo.laurie</t>
+  </si>
+  <si>
+    <t>chaplin.charles</t>
+  </si>
+  <si>
+    <t>gauger.sabine</t>
+  </si>
+  <si>
+    <t>serie.dexter</t>
+  </si>
+  <si>
+    <t>machado.chloe</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -522,10 +522,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -553,8 +553,8 @@
       <c r="A2">
         <v>20</v>
       </c>
-      <c r="B2">
-        <v>20</v>
+      <c r="B2" t="s">
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -563,7 +563,7 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>18</v>
@@ -582,8 +582,8 @@
       <c r="A3">
         <v>21</v>
       </c>
-      <c r="B3">
-        <v>21</v>
+      <c r="B3" t="s">
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -592,7 +592,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>18</v>
@@ -611,8 +611,8 @@
       <c r="A4">
         <v>22</v>
       </c>
-      <c r="B4">
-        <v>22</v>
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -621,7 +621,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>18</v>
@@ -640,8 +640,8 @@
       <c r="A5">
         <v>23</v>
       </c>
-      <c r="B5">
-        <v>23</v>
+      <c r="B5" t="s">
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -650,7 +650,7 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>18</v>
@@ -669,8 +669,8 @@
       <c r="A6">
         <v>24</v>
       </c>
-      <c r="B6">
-        <v>24</v>
+      <c r="B6" t="s">
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -679,7 +679,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
@@ -698,8 +698,8 @@
       <c r="A7">
         <v>25</v>
       </c>
-      <c r="B7">
-        <v>25</v>
+      <c r="B7" t="s">
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -708,7 +708,7 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>18</v>

</xml_diff>